<commit_message>
Added mod in Modellvergleich
</commit_message>
<xml_diff>
--- a/tables/Modellvergleich.xlsx
+++ b/tables/Modellvergleich.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t xml:space="preserve">Priorität für Modellauswahl: 1. Verfügbarkeit – 2. Lizenz – 3. Kosten – 4. Performance (spezifisch/allgemein)</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Datum</t>
   </si>
   <si>
+    <t xml:space="preserve">Mod</t>
+  </si>
+  <si>
     <t xml:space="preserve">Verfügbarkeit </t>
   </si>
   <si>
@@ -46,7 +49,7 @@
     <t xml:space="preserve">CORD</t>
   </si>
   <si>
-    <t xml:space="preserve">RVL-CLIP</t>
+    <t xml:space="preserve">RVLCLIP</t>
   </si>
   <si>
     <t xml:space="preserve">DocVQA</t>
@@ -61,6 +64,9 @@
     <t xml:space="preserve">aktuell</t>
   </si>
   <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">GCP/PythonAPI + Tutorials und Demos</t>
   </si>
   <si>
@@ -70,9 +76,6 @@
     <t xml:space="preserve">65$/1000pages</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">DocFormer base</t>
   </si>
   <si>
@@ -82,6 +85,9 @@
     <t xml:space="preserve">2021-09</t>
   </si>
   <si>
+    <t xml:space="preserve">VTL</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -231,6 +237,9 @@
     <t xml:space="preserve">2022-10</t>
   </si>
   <si>
+    <t xml:space="preserve">TL</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -257,6 +266,9 @@
   </si>
   <si>
     <t xml:space="preserve">Naver Clova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
   </si>
   <si>
     <r>
@@ -563,23 +575,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="72.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="71.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -594,6 +607,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -608,6 +622,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -636,331 +651,367 @@
       <c r="I5" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="J5" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="8" t="n">
+      <c r="F7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="8" t="n">
         <f aca="false"> AVERAGE(96.33)</f>
         <v>96.33</v>
       </c>
-      <c r="H7" s="8" t="n">
+      <c r="I7" s="8" t="n">
         <v>96.17</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>16</v>
+      <c r="J7" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="8" t="n">
+      <c r="G8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="8" t="n">
         <f aca="false"> AVERAGE(96.99)</f>
         <v>96.99</v>
       </c>
-      <c r="H8" s="8" t="n">
+      <c r="I8" s="8" t="n">
         <v>95.5</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>16</v>
+      <c r="J8" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="F9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="8" t="n">
         <f aca="false"> AVERAGE(94.95)</f>
         <v>94.95</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="I9" s="8" t="n">
         <v>95.25</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="J9" s="8" t="n">
         <v>78.08</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="8" t="n">
+      <c r="G10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="8" t="n">
         <f aca="false"> AVERAGE(96.01)</f>
         <v>96.01</v>
       </c>
-      <c r="H10" s="8" t="n">
+      <c r="I10" s="8" t="n">
         <v>95.64</v>
       </c>
-      <c r="I10" s="8" t="n">
+      <c r="J10" s="8" t="n">
         <v>78.8</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>29</v>
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="8" t="n">
         <f aca="false"> AVERAGE(96.56)</f>
         <v>96.56</v>
       </c>
-      <c r="H11" s="8" t="n">
+      <c r="I11" s="8" t="n">
         <v>95.44</v>
       </c>
-      <c r="I11" s="8" t="n">
+      <c r="J11" s="8" t="n">
         <v>78.76</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>29</v>
+        <v>37</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="8" t="n">
         <f aca="false"> AVERAGE(97.46)</f>
         <v>97.46</v>
       </c>
-      <c r="H12" s="8" t="n">
+      <c r="I12" s="8" t="n">
         <v>95.39</v>
       </c>
-      <c r="I12" s="8" t="n">
+      <c r="J12" s="8" t="n">
         <v>83.4</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="8" t="n">
+        <v>14</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="8" t="n">
         <v>72.7</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="8" t="n">
+        <v>23</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="8" t="n">
         <f aca="false"> AVERAGE(91.6)</f>
         <v>91.6</v>
       </c>
-      <c r="H14" s="8" t="n">
+      <c r="I14" s="8" t="n">
         <v>95.3</v>
       </c>
-      <c r="I14" s="8" t="n">
+      <c r="J14" s="8" t="n">
         <v>72.1</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>16</v>
+        <v>54</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="8" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="8" t="n">
         <f aca="false"> AVERAGE(97.58)</f>
         <v>97.58</v>
       </c>
-      <c r="H15" s="8" t="n">
+      <c r="I15" s="8" t="n">
         <v>96</v>
       </c>
-      <c r="I15" s="8" t="n">
+      <c r="J15" s="8" t="n">
         <v>84.7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>16</v>
+      <c r="D16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="8" t="n">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="8" t="n">
         <v>97.21</v>
       </c>
-      <c r="H16" s="8" t="n">
+      <c r="I16" s="8" t="n">
         <v>96.27</v>
       </c>
-      <c r="I16" s="8" t="n">
+      <c r="J16" s="8" t="n">
         <v>77.58</v>
       </c>
     </row>
@@ -971,9 +1022,10 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="8"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
@@ -982,9 +1034,10 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="8"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
@@ -993,9 +1046,10 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="8"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
@@ -1004,9 +1058,10 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="8"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
@@ -1015,9 +1070,10 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="8"/>
+      <c r="G21" s="5"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
@@ -1026,9 +1082,10 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="8"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
@@ -1037,9 +1094,10 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="8"/>
+      <c r="G23" s="5"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1171,20 +1229,20 @@
     <row r="151" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" display="https://github.com/shabie/docformer"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://github.com/shabie/docformer"/>
-    <hyperlink ref="D9" r:id="rId3" display="https://huggingface.co/microsoft/layoutlmv2-base-uncased"/>
-    <hyperlink ref="D10" r:id="rId4" display="https://huggingface.co/microsoft/layoutlmv2-large-uncased"/>
-    <hyperlink ref="D11" r:id="rId5" display="https://huggingface.co/microsoft/layoutlmv3-base"/>
-    <hyperlink ref="D12" r:id="rId6" display="https://huggingface.co/microsoft/layoutlmv3-large"/>
-    <hyperlink ref="D13" r:id="rId7" display="https://huggingface.co/microsoft/xdoc-base"/>
-    <hyperlink ref="D14" r:id="rId8" display="https://huggingface.co/naver-clova-ix/donut-base"/>
-    <hyperlink ref="D15" r:id="rId9" display="https://github.com/microsoft/i-Code/tree/main/i-Code-Doc"/>
-    <hyperlink ref="D16" r:id="rId10" display="https://github.com/PaddlePaddle/PaddleNLP/tree/develop/model_zoo/ernie-layout"/>
+    <hyperlink ref="E7" r:id="rId1" display="https://github.com/shabie/docformer"/>
+    <hyperlink ref="E8" r:id="rId2" display="https://github.com/shabie/docformer"/>
+    <hyperlink ref="E9" r:id="rId3" display="https://huggingface.co/microsoft/layoutlmv2-base-uncased"/>
+    <hyperlink ref="E10" r:id="rId4" display="https://huggingface.co/microsoft/layoutlmv2-large-uncased"/>
+    <hyperlink ref="E11" r:id="rId5" display="https://huggingface.co/microsoft/layoutlmv3-base"/>
+    <hyperlink ref="E12" r:id="rId6" display="https://huggingface.co/microsoft/layoutlmv3-large"/>
+    <hyperlink ref="E13" r:id="rId7" display="https://huggingface.co/microsoft/xdoc-base"/>
+    <hyperlink ref="E14" r:id="rId8" display="https://huggingface.co/naver-clova-ix/donut-base"/>
+    <hyperlink ref="E15" r:id="rId9" display="https://github.com/microsoft/i-Code/tree/main/i-Code-Doc"/>
+    <hyperlink ref="E16" r:id="rId10" display="https://github.com/PaddlePaddle/PaddleNLP/tree/develop/model_zoo/ernie-layout"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>